<commit_message>
Ending of Chapter 02.
</commit_message>
<xml_diff>
--- a/Resources/Exercise Files/Ch02/02 - Entering Data.xlsx
+++ b/Resources/Exercise Files/Ch02/02 - Entering Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennis Taylor\Desktop\Excel 2019 Desktop\Exercise Files\Ch02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://quintiles-my.sharepoint.com/personal/mdmuntaha_islam_iqvia_com/Documents/Documents/My Courses/Excel-Essential-Training/Resources/Exercise Files/Ch02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C258FC04-AEEB-4AC3-94CF-2B61188A6C76}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="10_ncr:8100000_{C258FC04-AEEB-4AC3-94CF-2B61188A6C76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6F3663D0-4625-4AFC-8696-0769E3778B9D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12351" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataEntry" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,252 @@
     <sheet name="Undo-Redo" sheetId="5" r:id="rId4"/>
     <sheet name="Save" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Islam, Md Muntaha EX1</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{95950F4F-1F8C-42C9-A6A1-AA0303DE220D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Islam, Md Muntaha EX1:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Autofilled.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{94F566C9-4255-4EB8-8E8A-C48DBCD8C8B1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Islam, Md Muntaha EX1:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Strings alined to left.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{DD40011B-4CA5-4D8F-A7A3-4B13B8286393}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Islam, Md Muntaha EX1:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Numbers alined to right.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{51745CDB-0150-4238-B7DA-C9A0E3618D74}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Islam, Md Muntaha EX1:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This autofill stops at 4 and then restarts.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{27758B6B-32F2-4A1C-BE72-12320C33D220}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Islam, Md Muntaha EX1:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Keep date columns a bit wider to find out if a date is invalid.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{5D00A2AB-B479-4BAB-9885-42E03FD8C9CB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Islam, Md Muntaha EX1:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Even after I put slashes, it changes to dash auto as that’s my pc's date system.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{C131FF7F-8C51-4862-B3D6-C4F54E2462B4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Islam, Md Muntaha EX1:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+am -&gt; AM</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{EAADB6A7-3E54-4FF2-AB9F-072257BD0C22}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Islam, Md Muntaha EX1:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+As it's invalid, it's alined to left, as a string.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{B8A58234-7314-4286-81B8-819B6C1FD322}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Islam, Md Muntaha EX1:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+100 days after day on B10.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="30">
   <si>
     <t>Sales</t>
   </si>
@@ -98,13 +333,34 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>32-11-22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +375,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -450,17 +725,151 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00FF00"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>120</v>
+      </c>
+      <c r="C2">
+        <v>160</v>
+      </c>
+      <c r="D2">
+        <v>190</v>
+      </c>
+      <c r="E2">
+        <v>220</v>
+      </c>
+      <c r="F2">
+        <v>240</v>
+      </c>
+      <c r="G2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>130</v>
+      </c>
+      <c r="D3">
+        <v>160</v>
+      </c>
+      <c r="E3">
+        <v>170</v>
+      </c>
+      <c r="F3">
+        <v>200</v>
+      </c>
+      <c r="G3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B10" s="1">
+        <v>44876</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.49236111111111108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B11" s="1">
+        <v>44876</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.49236111111111108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B13" s="1">
+        <f>B10+100</f>
+        <v>44976</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -473,9 +882,9 @@
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -495,7 +904,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -518,7 +927,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -541,12 +950,12 @@
         <v>360</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
@@ -557,7 +966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
@@ -568,7 +977,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
@@ -579,7 +988,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
         <v>14</v>
       </c>
@@ -604,16 +1013,16 @@
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.23046875" style="10"/>
-    <col min="2" max="2" width="10.3828125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.84375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="9.84375" customWidth="1"/>
-    <col min="5" max="9" width="9.23046875" style="10"/>
+    <col min="1" max="1" width="9.26953125" style="10"/>
+    <col min="2" max="2" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" customWidth="1"/>
+    <col min="5" max="9" width="9.26953125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B1" s="6" t="s">
         <v>21</v>
       </c>
@@ -621,7 +1030,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B2" s="1">
         <v>43322</v>
       </c>
@@ -629,899 +1038,899 @@
         <v>0.69652777777777775</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3" s="10"/>
       <c r="D3" s="10"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4" s="10"/>
       <c r="D4" s="10"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" s="10"/>
       <c r="D5" s="10"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6" s="10"/>
       <c r="D6" s="10"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7" s="10"/>
       <c r="D7" s="10"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" s="10"/>
       <c r="D8" s="10"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9" s="10"/>
       <c r="D9" s="10"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10" s="10"/>
       <c r="D10" s="10"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B11" s="10"/>
       <c r="D11" s="10"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12" s="10"/>
       <c r="D12" s="10"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13" s="10"/>
       <c r="D13" s="10"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14" s="10"/>
       <c r="D14" s="10"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B15" s="10"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B16" s="10"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="10"/>
       <c r="D17" s="10"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="10"/>
       <c r="D18" s="10"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="10"/>
       <c r="D19" s="10"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" s="10"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B21" s="10"/>
       <c r="D21" s="10"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B22" s="10"/>
       <c r="D22" s="10"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B23" s="10"/>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B24" s="10"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B25" s="10"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B26" s="10"/>
       <c r="D26" s="10"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B27" s="10"/>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B28" s="10"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B29" s="10"/>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B30" s="10"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B31" s="10"/>
       <c r="D31" s="10"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B32" s="10"/>
       <c r="D32" s="10"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B33" s="10"/>
       <c r="D33" s="10"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B34" s="10"/>
       <c r="D34" s="10"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B35" s="10"/>
       <c r="D35" s="10"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B36" s="10"/>
       <c r="D36" s="10"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B37" s="10"/>
       <c r="D37" s="10"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B38" s="10"/>
       <c r="D38" s="10"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B39" s="10"/>
       <c r="D39" s="10"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B40" s="10"/>
       <c r="D40" s="10"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B41" s="10"/>
       <c r="D41" s="10"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B42" s="10"/>
       <c r="D42" s="10"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B43" s="10"/>
       <c r="D43" s="10"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B44" s="10"/>
       <c r="D44" s="10"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B45" s="10"/>
       <c r="D45" s="10"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B46" s="10"/>
       <c r="D46" s="10"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B47" s="10"/>
       <c r="D47" s="10"/>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B48" s="10"/>
       <c r="D48" s="10"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B49" s="10"/>
       <c r="D49" s="10"/>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B50" s="10"/>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B51" s="10"/>
       <c r="D51" s="10"/>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B52" s="10"/>
       <c r="D52" s="10"/>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B53" s="10"/>
       <c r="D53" s="10"/>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B54" s="10"/>
       <c r="D54" s="10"/>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B55" s="10"/>
       <c r="D55" s="10"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B56" s="10"/>
       <c r="D56" s="10"/>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B57" s="10"/>
       <c r="D57" s="10"/>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B58" s="10"/>
       <c r="D58" s="10"/>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B59" s="10"/>
       <c r="D59" s="10"/>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B60" s="10"/>
       <c r="D60" s="10"/>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B61" s="10"/>
       <c r="D61" s="10"/>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B62" s="10"/>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B63" s="10"/>
       <c r="D63" s="10"/>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B64" s="10"/>
       <c r="D64" s="10"/>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B65" s="10"/>
       <c r="D65" s="10"/>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B66" s="10"/>
       <c r="D66" s="10"/>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B67" s="10"/>
       <c r="D67" s="10"/>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B68" s="10"/>
       <c r="D68" s="10"/>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B69" s="10"/>
       <c r="D69" s="10"/>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B70" s="10"/>
       <c r="D70" s="10"/>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B71" s="10"/>
       <c r="D71" s="10"/>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B72" s="10"/>
       <c r="D72" s="10"/>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B73" s="10"/>
       <c r="D73" s="10"/>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B74" s="10"/>
       <c r="D74" s="10"/>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B75" s="10"/>
       <c r="D75" s="10"/>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B76" s="10"/>
       <c r="D76" s="10"/>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B77" s="10"/>
       <c r="D77" s="10"/>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B78" s="10"/>
       <c r="D78" s="10"/>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="79" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B79" s="10"/>
       <c r="D79" s="10"/>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="80" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B80" s="10"/>
       <c r="D80" s="10"/>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B81" s="10"/>
       <c r="D81" s="10"/>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B82" s="10"/>
       <c r="D82" s="10"/>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B83" s="10"/>
       <c r="D83" s="10"/>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B84" s="10"/>
       <c r="D84" s="10"/>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B85" s="10"/>
       <c r="D85" s="10"/>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B86" s="10"/>
       <c r="D86" s="10"/>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B87" s="10"/>
       <c r="D87" s="10"/>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B88" s="10"/>
       <c r="D88" s="10"/>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B89" s="10"/>
       <c r="D89" s="10"/>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B90" s="10"/>
       <c r="D90" s="10"/>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B91" s="10"/>
       <c r="D91" s="10"/>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B92" s="10"/>
       <c r="D92" s="10"/>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B93" s="10"/>
       <c r="D93" s="10"/>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B94" s="10"/>
       <c r="D94" s="10"/>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B95" s="10"/>
       <c r="D95" s="10"/>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B96" s="10"/>
       <c r="D96" s="10"/>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B97" s="10"/>
       <c r="D97" s="10"/>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B98" s="10"/>
       <c r="D98" s="10"/>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B99" s="10"/>
       <c r="D99" s="10"/>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B100" s="10"/>
       <c r="D100" s="10"/>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B101" s="10"/>
       <c r="D101" s="10"/>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B102" s="10"/>
       <c r="D102" s="10"/>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B103" s="10"/>
       <c r="D103" s="10"/>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B104" s="10"/>
       <c r="D104" s="10"/>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B105" s="10"/>
       <c r="D105" s="10"/>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B106" s="10"/>
       <c r="D106" s="10"/>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B107" s="10"/>
       <c r="D107" s="10"/>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B108" s="10"/>
       <c r="D108" s="10"/>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B109" s="10"/>
       <c r="D109" s="10"/>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B110" s="10"/>
       <c r="D110" s="10"/>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B111" s="10"/>
       <c r="D111" s="10"/>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B112" s="10"/>
       <c r="D112" s="10"/>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B113" s="10"/>
       <c r="D113" s="10"/>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B114" s="10"/>
       <c r="D114" s="10"/>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B115" s="10"/>
       <c r="D115" s="10"/>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B116" s="10"/>
       <c r="D116" s="10"/>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B117" s="10"/>
       <c r="D117" s="10"/>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B118" s="10"/>
       <c r="D118" s="10"/>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B119" s="10"/>
       <c r="D119" s="10"/>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B120" s="10"/>
       <c r="D120" s="10"/>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B121" s="10"/>
       <c r="D121" s="10"/>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B122" s="10"/>
       <c r="D122" s="10"/>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B123" s="10"/>
       <c r="D123" s="10"/>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B124" s="10"/>
       <c r="D124" s="10"/>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="125" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B125" s="10"/>
       <c r="D125" s="10"/>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B126" s="10"/>
       <c r="D126" s="10"/>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B127" s="10"/>
       <c r="D127" s="10"/>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B128" s="10"/>
       <c r="D128" s="10"/>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B129" s="10"/>
       <c r="D129" s="10"/>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B130" s="10"/>
       <c r="D130" s="10"/>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B131" s="10"/>
       <c r="D131" s="10"/>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B132" s="10"/>
       <c r="D132" s="10"/>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B133" s="10"/>
       <c r="D133" s="10"/>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B134" s="10"/>
       <c r="D134" s="10"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B135" s="10"/>
       <c r="D135" s="10"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B136" s="10"/>
       <c r="D136" s="10"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B137" s="10"/>
       <c r="D137" s="10"/>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B138" s="10"/>
       <c r="D138" s="10"/>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B139" s="10"/>
       <c r="D139" s="10"/>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B140" s="10"/>
       <c r="D140" s="10"/>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B141" s="10"/>
       <c r="D141" s="10"/>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B142" s="10"/>
       <c r="D142" s="10"/>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B143" s="10"/>
       <c r="D143" s="10"/>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B144" s="10"/>
       <c r="D144" s="10"/>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B145" s="10"/>
       <c r="D145" s="10"/>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="146" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B146" s="10"/>
       <c r="D146" s="10"/>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="147" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B147" s="10"/>
       <c r="D147" s="10"/>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="148" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B148" s="10"/>
       <c r="D148" s="10"/>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="149" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B149" s="10"/>
       <c r="D149" s="10"/>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="150" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B150" s="10"/>
       <c r="D150" s="10"/>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="151" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B151" s="10"/>
       <c r="D151" s="10"/>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="152" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B152" s="10"/>
       <c r="D152" s="10"/>
     </row>
-    <row r="153" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="153" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B153" s="10"/>
       <c r="D153" s="10"/>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="154" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B154" s="10"/>
       <c r="D154" s="10"/>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="155" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B155" s="10"/>
       <c r="D155" s="10"/>
     </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="156" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B156" s="10"/>
       <c r="D156" s="10"/>
     </row>
-    <row r="157" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="157" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B157" s="10"/>
       <c r="D157" s="10"/>
     </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="158" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B158" s="10"/>
       <c r="D158" s="10"/>
     </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="159" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B159" s="10"/>
       <c r="D159" s="10"/>
     </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="160" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B160" s="10"/>
       <c r="D160" s="10"/>
     </row>
-    <row r="161" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="161" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B161" s="10"/>
       <c r="D161" s="10"/>
     </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="162" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B162" s="10"/>
       <c r="D162" s="10"/>
     </row>
-    <row r="163" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="163" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B163" s="10"/>
       <c r="D163" s="10"/>
     </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="164" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B164" s="10"/>
       <c r="D164" s="10"/>
     </row>
-    <row r="165" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="165" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B165" s="10"/>
       <c r="D165" s="10"/>
     </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="166" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B166" s="10"/>
       <c r="D166" s="10"/>
     </row>
-    <row r="167" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="167" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B167" s="10"/>
       <c r="D167" s="10"/>
     </row>
-    <row r="168" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="168" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B168" s="10"/>
       <c r="D168" s="10"/>
     </row>
-    <row r="169" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="169" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B169" s="10"/>
       <c r="D169" s="10"/>
     </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="170" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B170" s="10"/>
       <c r="D170" s="10"/>
     </row>
-    <row r="171" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="171" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B171" s="10"/>
       <c r="D171" s="10"/>
     </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="172" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B172" s="10"/>
       <c r="D172" s="10"/>
     </row>
-    <row r="173" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="173" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B173" s="10"/>
       <c r="D173" s="10"/>
     </row>
-    <row r="174" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="174" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B174" s="10"/>
       <c r="D174" s="10"/>
     </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="175" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B175" s="10"/>
       <c r="D175" s="10"/>
     </row>
-    <row r="176" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="176" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B176" s="10"/>
       <c r="D176" s="10"/>
     </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="177" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B177" s="10"/>
       <c r="D177" s="10"/>
     </row>
-    <row r="178" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="178" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B178" s="10"/>
       <c r="D178" s="10"/>
     </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="179" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B179" s="10"/>
       <c r="D179" s="10"/>
     </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="180" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B180" s="10"/>
       <c r="D180" s="10"/>
     </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="181" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B181" s="10"/>
       <c r="D181" s="10"/>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="182" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B182" s="10"/>
       <c r="D182" s="10"/>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="183" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B183" s="10"/>
       <c r="D183" s="10"/>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="184" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B184" s="10"/>
       <c r="D184" s="10"/>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="185" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B185" s="11"/>
       <c r="D185" s="11"/>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="186" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B186" s="11"/>
       <c r="D186" s="11"/>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B187" s="11"/>
       <c r="D187" s="11"/>
     </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="188" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B188" s="11"/>
       <c r="D188" s="11"/>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="189" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B189" s="11"/>
       <c r="D189" s="11"/>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="190" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B190" s="11"/>
       <c r="D190" s="11"/>
     </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="191" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B191" s="11"/>
       <c r="D191" s="11"/>
     </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="192" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B192" s="11"/>
       <c r="D192" s="11"/>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B193" s="11"/>
       <c r="D193" s="11"/>
     </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="194" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B194" s="11"/>
       <c r="D194" s="11"/>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B195" s="11"/>
       <c r="D195" s="11"/>
     </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="196" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B196" s="11"/>
       <c r="D196" s="11"/>
     </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="197" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B197" s="11"/>
       <c r="D197" s="11"/>
     </row>
-    <row r="198" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="198" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B198" s="11"/>
       <c r="D198" s="11"/>
     </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="199" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B199" s="11"/>
       <c r="D199" s="11"/>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B200" s="11"/>
       <c r="D200" s="11"/>
     </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B201" s="11"/>
       <c r="D201" s="11"/>
     </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="202" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B202" s="11"/>
       <c r="D202" s="11"/>
     </row>
-    <row r="203" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="203" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B203" s="11"/>
       <c r="D203" s="11"/>
     </row>
-    <row r="204" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="204" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B204" s="11"/>
       <c r="D204" s="11"/>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B205" s="11"/>
       <c r="D205" s="11"/>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B206" s="11"/>
       <c r="D206" s="11"/>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B207" s="11"/>
       <c r="D207" s="11"/>
     </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B208" s="11"/>
       <c r="D208" s="11"/>
     </row>
-    <row r="209" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="209" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B209" s="11"/>
       <c r="D209" s="11"/>
     </row>
-    <row r="210" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="210" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B210" s="11"/>
       <c r="D210" s="11"/>
     </row>
-    <row r="211" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="211" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B211" s="11"/>
       <c r="D211" s="11"/>
     </row>
-    <row r="212" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="212" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B212" s="11"/>
       <c r="D212" s="11"/>
     </row>
-    <row r="213" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="213" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B213" s="11"/>
       <c r="D213" s="11"/>
     </row>
-    <row r="214" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="214" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B214" s="11"/>
       <c r="D214" s="11"/>
     </row>
-    <row r="215" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="215" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B215" s="11"/>
       <c r="D215" s="11"/>
     </row>
-    <row r="216" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="216" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B216" s="11"/>
       <c r="D216" s="11"/>
     </row>
-    <row r="217" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="217" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B217" s="11"/>
       <c r="D217" s="11"/>
     </row>
-    <row r="218" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="218" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B218" s="11"/>
       <c r="D218" s="11"/>
     </row>
-    <row r="219" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="219" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B219" s="11"/>
       <c r="D219" s="11"/>
     </row>
-    <row r="220" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="220" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B220" s="11"/>
       <c r="D220" s="11"/>
     </row>
-    <row r="221" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="221" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B221" s="11"/>
       <c r="D221" s="11"/>
     </row>
-    <row r="222" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="222" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B222" s="11"/>
       <c r="D222" s="11"/>
     </row>
-    <row r="223" spans="2:4" x14ac:dyDescent="0.4">
+    <row r="223" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B223" s="11"/>
       <c r="D223" s="11"/>
     </row>
@@ -1539,9 +1948,9 @@
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
@@ -1561,7 +1970,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1584,7 +1993,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1607,7 +2016,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -1626,9 +2035,9 @@
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
@@ -1648,7 +2057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1671,7 +2080,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1694,7 +2103,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>

</xml_diff>